<commit_message>
Updated Excel file with Sq Meter to Sq Feet conversion
Updated Excel file with Sq Meter to Sq Feet conversion
</commit_message>
<xml_diff>
--- a/Electrical Demand Calculation.xlsx
+++ b/Electrical Demand Calculation.xlsx
@@ -5,33 +5,34 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kphillips\Dropbox\KP Phillips Work Backup\Hypar\Service Demand Calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kphillips\Desktop\Hypar-Excel-Functions-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C317E-E477-466C-8098-9D66644D81E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015938BD-B1FB-4F63-9362-FFFB4F1172F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="-19200" windowWidth="20055" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4230" yWindow="330" windowWidth="23535" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="INPUT.01.Building.Area.SF">Sheet1!$B$3</definedName>
-    <definedName name="INPUT.02.Voltage">Sheet1!$B$4</definedName>
-    <definedName name="INPUT.03.Phase">Sheet1!$B$5</definedName>
-    <definedName name="INPUT.04.Lighting.Loads.kVA_SF">Sheet1!$C$9</definedName>
-    <definedName name="INPUT.05.Receptacle.Loads.kVA_SF">Sheet1!$C$11</definedName>
-    <definedName name="INPUT.06.Technology.Loads.kVA_SF">Sheet1!$C$13</definedName>
-    <definedName name="INPUT.07.Plumbing.FireProtection.Loads.kVA_SF">Sheet1!$C$15</definedName>
-    <definedName name="INPUT.08.HVAC.Loads.kVA_SF">Sheet1!$C$17</definedName>
-    <definedName name="INPUT.09.General.Ventilation.Loads.kVA_SF">Sheet1!$C$19</definedName>
-    <definedName name="INPUT.10.Equipment.Pump.Loads.kVA_SF">Sheet1!$C$21</definedName>
-    <definedName name="INPUT.11.Misc.Loads.kVA">Sheet1!$D$23</definedName>
-    <definedName name="INPUT.12.Percent.Future.Expansion">Sheet1!$B$27</definedName>
-    <definedName name="INPUT.13.Percent.Demand.Of.Connected">Sheet1!$B$31</definedName>
-    <definedName name="OUTPUT.14.Total.Connected.Load">Sheet1!$D$29</definedName>
-    <definedName name="OUTPUT.15.Estimated.Demand.Load.kVA">Sheet1!$D$31</definedName>
-    <definedName name="OUTPUT.16.Estimated.Demand.Load.Amps">Sheet1!$D$33</definedName>
+    <definedName name="INPUT.00.Convert.SM.to.SF">Sheet1!$B$3</definedName>
+    <definedName name="INPUT.01.Building.Area">Sheet1!$B$4</definedName>
+    <definedName name="INPUT.02.Voltage">Sheet1!$B$5</definedName>
+    <definedName name="INPUT.03.Phase">Sheet1!$B$6</definedName>
+    <definedName name="INPUT.04.Lighting.Loads.kVA_SF">Sheet1!$C$10</definedName>
+    <definedName name="INPUT.05.Receptacle.Loads.kVA_SF">Sheet1!$C$12</definedName>
+    <definedName name="INPUT.06.Technology.Loads.kVA_SF">Sheet1!$C$14</definedName>
+    <definedName name="INPUT.07.Plumbing.FireProtection.Loads.kVA_SF">Sheet1!$C$16</definedName>
+    <definedName name="INPUT.08.HVAC.Loads.kVA_SF">Sheet1!$C$18</definedName>
+    <definedName name="INPUT.09.General.Ventilation.Loads.kVA_SF">Sheet1!$C$20</definedName>
+    <definedName name="INPUT.10.Equipment.Pump.Loads.kVA_SF">Sheet1!$C$22</definedName>
+    <definedName name="INPUT.11.Misc.Loads.kVA">Sheet1!$D$24</definedName>
+    <definedName name="INPUT.12.Percent.Future.Expansion">Sheet1!$B$28</definedName>
+    <definedName name="INPUT.13.Percent.Demand.Of.Connected">Sheet1!$B$32</definedName>
+    <definedName name="OUTPUT.14.Total.Connected.Load">Sheet1!$D$30</definedName>
+    <definedName name="OUTPUT.15.Estimated.Demand.Load.kVA">Sheet1!$D$32</definedName>
+    <definedName name="OUTPUT.16.Estimated.Demand.Load.Amps">Sheet1!$D$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -104,9 +105,6 @@
     <t>Amps</t>
   </si>
   <si>
-    <t>SF</t>
-  </si>
-  <si>
     <t>kVA/SF</t>
   </si>
   <si>
@@ -129,6 +127,9 @@
   </si>
   <si>
     <t>~ Demand Amps @</t>
+  </si>
+  <si>
+    <t>Convert Sq Meters to Sq Feet (1=YES, 0=NO)</t>
   </si>
 </sst>
 </file>
@@ -300,19 +301,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -369,6 +357,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -376,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -402,25 +401,24 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,9 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -712,358 +712,372 @@
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
+      <c r="A3" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="19">
-        <v>125000</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>10</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="21">
-        <v>480</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="31">
+        <v>256660</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="23" t="s">
-        <v>11</v>
+      <c r="D4" s="32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="21">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="B5" s="19">
+        <v>480</v>
       </c>
       <c r="C5" s="7"/>
+      <c r="D5" s="20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="19">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
       <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="28">
+        <v>1.2</v>
+      </c>
+      <c r="D10" s="11">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C10, "m2", "ft2")*$B$4/1000,C10*$B$4/1000)</f>
+        <v>3315.1982970632607</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="31">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="11">
-        <f>C9*$B$3/1000</f>
-        <v>150</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C12, "m2", "ft2")*$B$4/1000,C12*$B$4/1000)</f>
+        <v>4143.9978713290757</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="30">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C14, "m2", "ft2")*$B$4/1000,C14*$B$4/1000)</f>
+        <v>4143.9978713290757</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="30">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C16, "m2", "ft2")*$B$4/1000,C16*$B$4/1000)</f>
+        <v>2762.6652475527171</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="30">
+        <v>10</v>
+      </c>
+      <c r="D18" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C18, "m2", "ft2")*$B$4/1000,C18*$B$4/1000)</f>
+        <v>27626.652475527175</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="D11" s="12">
-        <f>C11*$B$3/1000</f>
-        <v>187.5</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="D13" s="12">
-        <f>C13*$B$3/1000</f>
-        <v>187.5</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="33">
+      <c r="B20" s="6"/>
+      <c r="C20" s="30">
+        <v>2</v>
+      </c>
+      <c r="D20" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C20, "m2", "ft2")*$B$4/1000,C20*$B$4/1000)</f>
+        <v>5525.3304951054342</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="30">
         <v>1</v>
       </c>
-      <c r="D15" s="12">
-        <f>C15*$B$3/1000</f>
-        <v>125</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="33">
-        <v>10</v>
-      </c>
-      <c r="D17" s="12">
-        <f>C17*$B$3/1000</f>
-        <v>1250</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="33">
-        <v>2</v>
-      </c>
-      <c r="D19" s="12">
-        <f>C19*$B$3/1000</f>
-        <v>250</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="33">
-        <v>1</v>
-      </c>
-      <c r="D21" s="12">
-        <f>C21*$B$3/1000</f>
-        <v>125</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="D22" s="12">
+        <f>IF(INPUT.00.Convert.SM.to.SF=1,CONVERT(C22, "m2", "ft2")*$B$4/1000,C22*$B$4/1000)</f>
+        <v>2762.6652475527171</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="16">
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="16">
         <v>300</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="18">
-        <f>SUM(D9:D24)</f>
-        <v>2575</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
+      <c r="D26" s="18">
+        <f>SUM(D10:D25)</f>
+        <v>50580.507505459456</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B28" s="17">
         <v>0.2</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="18">
-        <f>D25*B27</f>
-        <v>515</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
+      <c r="D28" s="18">
+        <f>D26*B28</f>
+        <v>10116.101501091893</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="26">
-        <f>SUM(D25:D27)</f>
-        <v>3090</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="10"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23">
+        <f>SUM(D26:D28)</f>
+        <v>60696.609006551349</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B32" s="25">
         <v>0.8</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C32" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="29">
-        <f>D29*B31</f>
-        <v>2472</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
+      <c r="D32" s="26">
+        <f>D30*B32</f>
+        <v>48557.287205241082</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="25">
-        <f>B4</f>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="22">
+        <f>B5</f>
         <v>480</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="29">
-        <f>IF( B5=3, (D31/(SQRT(3)*B33))*1000, IF( B5=2, (D31/(B33))*1000, 0 ))</f>
-        <v>2973.353886326573</v>
-      </c>
-      <c r="E33" s="27" t="s">
+      <c r="C34" s="22"/>
+      <c r="D34" s="26">
+        <f>IF( B6=3, (D32/(SQRT(3)*B34))*1000, IF( B6=2, (D32/(B34))*1000, 0 ))</f>
+        <v>58405.339248049822</v>
+      </c>
+      <c r="E34" s="24" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>